<commit_message>
Check register for project as officer
</commit_message>
<xml_diff>
--- a/sc2002/src/main/resources/ManagerList.xlsx
+++ b/sc2002/src/main/resources/ManagerList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/hu0037ng_e_ntu_edu_sg/Documents/SC4079 - Final Year Project/SC2002/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\NTUWorkspace\Y1 Y2\Object Oriented Design &amp; Programming\project\sc2002\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_F25DC773A252ABDACC1048D321184AB85ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AED78119-22A7-4087-8472-22F30669F0DB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B95C361-391E-4536-84C2-5059824F0772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4057" yWindow="5932" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41490" yWindow="8400" windowWidth="19200" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Jessica</t>
   </si>
   <si>
-    <t>T8765432F</t>
-  </si>
-  <si>
     <t>S5678901G</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -381,12 +381,12 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,38 +403,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>26</v>
       </c>
       <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>